<commit_message>
Added the code for common function
</commit_message>
<xml_diff>
--- a/tests/artifact/data/AddProductPage.data.xlsx
+++ b/tests/artifact/data/AddProductPage.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="284">
   <si>
     <t>login.screen</t>
   </si>
@@ -857,17 +857,47 @@
   </si>
   <si>
     <t>(//*[text()='Save'])[2]</t>
+  </si>
+  <si>
+    <t>columnBusiness</t>
+  </si>
+  <si>
+    <t>//body/div//section//div//div[3]//table//tr/td[1]</t>
+  </si>
+  <si>
+    <t>columnName3</t>
+  </si>
+  <si>
+    <t>//table[@id='list-Business']//div[contains(text(),'Name')]</t>
+  </si>
+  <si>
+    <t>columnName1</t>
+  </si>
+  <si>
+    <t>//table[@id='</t>
+  </si>
+  <si>
+    <t>columnName2</t>
+  </si>
+  <si>
+    <t>]//div[contains(text(),'Name')]</t>
+  </si>
+  <si>
+    <t>columnName</t>
+  </si>
+  <si>
+    <t>list-Business'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -920,51 +950,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -982,7 +967,70 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -996,54 +1044,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1058,7 +1060,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1073,7 +1103,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1085,19 +1187,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1109,151 +1277,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1283,16 +1313,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1300,8 +1330,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1322,16 +1361,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1354,17 +1393,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1384,148 +1414,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1563,52 +1593,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1971,10 +2001,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C143"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="B127" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -3132,6 +3162,46 @@
         <v>273</v>
       </c>
     </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>

<commit_message>
Modification to the common function
</commit_message>
<xml_diff>
--- a/tests/artifact/data/AddProductPage.data.xlsx
+++ b/tests/artifact/data/AddProductPage.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="293">
   <si>
     <t>login.screen</t>
   </si>
@@ -196,7 +196,7 @@
     <t>org.workflow</t>
   </si>
   <si>
-    <t>//*[text()='Workflow']</t>
+    <t>//span[normalize-space()='Workflow']</t>
   </si>
   <si>
     <t>org.transactions</t>
@@ -553,7 +553,7 @@
     <t>click.Business</t>
   </si>
   <si>
-    <t>//*[text()='Business']</t>
+    <t>//*[text()='Audit Logs']</t>
   </si>
   <si>
     <t>click.addNewProduct</t>
@@ -859,10 +859,16 @@
     <t>(//*[text()='Save'])[2]</t>
   </si>
   <si>
+    <t>columnBusiness1</t>
+  </si>
+  <si>
+    <t>//body/div//section//div//div[3]//table//tr/td[1]</t>
+  </si>
+  <si>
     <t>columnBusiness</t>
   </si>
   <si>
-    <t>//body/div//section//div//div[3]//table//tr/td[1]</t>
+    <t>//body/div/main/section/div/table/tbody/tr/td[1]</t>
   </si>
   <si>
     <t>columnName3</t>
@@ -883,10 +889,31 @@
     <t>]//div[contains(text(),'Name')]</t>
   </si>
   <si>
+    <t>list-Business'</t>
+  </si>
+  <si>
     <t>columnName</t>
   </si>
   <si>
-    <t>list-Business'</t>
+    <t>Activity'</t>
+  </si>
+  <si>
+    <t>click.Admin</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Administration']</t>
+  </si>
+  <si>
+    <t>validate.AuditLogsPage</t>
+  </si>
+  <si>
+    <t>/html[1]/body[1]/div[1]/main[1]/section[1]/div[1]/div[1]</t>
+  </si>
+  <si>
+    <t>click.AuditLogs</t>
+  </si>
+  <si>
+    <t>(//span[normalize-space()='Audit Logs'])[1]</t>
   </si>
 </sst>
 </file>
@@ -2001,10 +2028,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="B127" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -3202,159 +3229,221 @@
         <v>283</v>
       </c>
     </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="12" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="18" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="16" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="15" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A25,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="27" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="33" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A26,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="28" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="34" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="29" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="30" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="36" stopIfTrue="1">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="5" priority="37" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="38">
+      <formula>LEN(TRIM(B26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="beginsWith" dxfId="3" priority="27" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A27,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="28" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="29" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="30" stopIfTrue="1">
+      <formula>LEN(TRIM(A27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
     <cfRule type="expression" dxfId="5" priority="31" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="4" priority="32">
-      <formula>LEN(TRIM(B26))&gt;0</formula>
+      <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
+  <conditionalFormatting sqref="A28">
     <cfRule type="beginsWith" dxfId="3" priority="21" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A27,LEN("//"))="//"</formula>
+      <formula>LEFT(A28,LEN("//"))="//"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="22" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
+      <formula>LEFT(A28,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A28,LEN("nexial."))="nexial."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="0" priority="24" stopIfTrue="1">
-      <formula>LEN(TRIM(A27))&gt;0</formula>
+      <formula>LEN(TRIM(A28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
+  <conditionalFormatting sqref="B28">
     <cfRule type="expression" dxfId="5" priority="25" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
     <cfRule type="notContainsBlanks" dxfId="4" priority="26">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
+      <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="beginsWith" dxfId="3" priority="15" stopIfTrue="1" operator="equal" text="//">
-      <formula>LEFT(A28,LEN("//"))="//"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="16" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A28,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A28,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="18" stopIfTrue="1">
-      <formula>LEN(TRIM(A28))&gt;0</formula>
+  <conditionalFormatting sqref="A150">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A150))&gt;0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A150,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A150,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A150,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
+  <conditionalFormatting sqref="B150">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+      <formula>LEN(TRIM(B150))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
-      <formula>LEN(TRIM(B28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="33" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="39" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="34" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="40" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="35" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="36" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="42" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A91">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A85))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A85,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A85,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A85,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="43" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="44">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B91">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="12">
       <formula>LEN(TRIM(B85))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E128 B92:B128 B41:B84 B29:B39 B129:E1048576">
-    <cfRule type="expression" dxfId="5" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E128 B92:B128 B41:B84 B29:B39 B129:E149 C150:E150 B151:E1048576">
+    <cfRule type="expression" dxfId="5" priority="49" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="52">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A29:A84 A92:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="39" stopIfTrue="1" operator="equal" text="//">
+  <conditionalFormatting sqref="A4:A24 A29:A84 A92:A149 A151:A1048576">
+    <cfRule type="beginsWith" dxfId="3" priority="45" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A4,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="40" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="46" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="47" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="42" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="48" stopIfTrue="1">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>